<commit_message>
Ensured all integers have a float of at least .0
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/3000.xlsx
+++ b/database/AN_ep/expdata/3000.xlsx
@@ -68,8 +68,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -152,13 +153,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -181,7 +186,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,11 +223,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>-0.6</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -234,7 +239,7 @@
       <c r="E2" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -250,11 +255,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>-0.53</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -266,7 +271,7 @@
       <c r="E3" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -282,11 +287,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>-0.46</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -298,7 +303,7 @@
       <c r="E4" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G4" s="0" t="s">
@@ -314,11 +319,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>-0.39</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -330,7 +335,7 @@
       <c r="E5" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G5" s="0" t="s">
@@ -346,11 +351,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>-0.32</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -362,7 +367,7 @@
       <c r="E6" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -378,11 +383,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>-0.25</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -394,7 +399,7 @@
       <c r="E7" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G7" s="0" t="s">
@@ -410,11 +415,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>-0.18</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -426,7 +431,7 @@
       <c r="E8" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -442,11 +447,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>-0.11</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -458,7 +463,7 @@
       <c r="E9" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -474,11 +479,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>-0.0399999999999999</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -490,7 +495,7 @@
       <c r="E10" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -510,7 +515,7 @@
       <c r="A11" s="0" t="n">
         <v>0.03</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -522,7 +527,7 @@
       <c r="E11" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -542,7 +547,7 @@
       <c r="A12" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -554,7 +559,7 @@
       <c r="E12" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -574,7 +579,7 @@
       <c r="A13" s="0" t="n">
         <v>0.169999999999999</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -586,7 +591,7 @@
       <c r="E13" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G13" s="0" t="s">
@@ -602,11 +607,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.239999999999999</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -618,7 +623,7 @@
       <c r="E14" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -634,11 +639,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>0.309999999999999</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -650,7 +655,7 @@
       <c r="E15" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G15" s="0" t="s">
@@ -666,11 +671,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0.379999999999999</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -682,7 +687,7 @@
       <c r="E16" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -698,11 +703,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0.45</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -714,7 +719,7 @@
       <c r="E17" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -730,11 +735,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>0.52</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -746,7 +751,7 @@
       <c r="E18" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G18" s="0" t="s">
@@ -762,11 +767,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>0.59</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -778,7 +783,7 @@
       <c r="E19" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
         <v>63</v>
       </c>
       <c r="G19" s="0" t="s">

</xml_diff>